<commit_message>
investiture soft anim - pewter bar - metal grinder
</commit_message>
<xml_diff>
--- a/.develop/ModAdditions.xlsx
+++ b/.develop/ModAdditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Documents\My Games\Terraria\tModLoader\ModSources\AllomancyMOD\.develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C370C1-3B54-47F8-B7C1-24C57DD1FB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5E838-C388-4E08-80A0-2F525A2518AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -703,16 +703,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1033,9 +1028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828CD007-B033-468F-8ADE-6460DAA113A1}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D43" sqref="D43"/>
+      <selection pane="topRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,7 +1067,7 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1102,7 +1097,7 @@
       <c r="P1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>108</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -1110,55 +1105,55 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="D2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2">
         <v>16</v>
       </c>
-      <c r="H2" s="5">
-        <v>1</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" s="5">
-        <v>0</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="5">
+      <c r="J2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>5</v>
       </c>
       <c r="R2" t="s">
@@ -1175,13 +1170,13 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G3">
@@ -1193,13 +1188,13 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M3">
@@ -1211,7 +1206,7 @@
       <c r="O3" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
@@ -1228,13 +1223,13 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G4">
@@ -1246,13 +1241,13 @@
       <c r="I4" t="s">
         <v>104</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M4">
@@ -1264,7 +1259,7 @@
       <c r="O4" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
@@ -1281,13 +1276,13 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G5">
@@ -1299,13 +1294,13 @@
       <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M5">
@@ -1317,7 +1312,7 @@
       <c r="O5" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
@@ -1334,13 +1329,13 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G6">
@@ -1352,13 +1347,13 @@
       <c r="I6" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M6">
@@ -1370,7 +1365,7 @@
       <c r="O6" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
@@ -1390,13 +1385,13 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G7">
@@ -1408,13 +1403,13 @@
       <c r="I7" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M7">
@@ -1426,7 +1421,7 @@
       <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="P7" s="8">
+      <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
@@ -1446,13 +1441,13 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G8">
@@ -1464,13 +1459,13 @@
       <c r="I8" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M8">
@@ -1482,7 +1477,7 @@
       <c r="O8" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
@@ -1502,13 +1497,13 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G9">
@@ -1517,16 +1512,16 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J9" s="3" t="s">
+      <c r="I9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M9">
@@ -1535,10 +1530,10 @@
       <c r="N9" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P9" s="5">
+      <c r="O9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
@@ -1558,13 +1553,13 @@
       <c r="C10" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G10">
@@ -1576,13 +1571,13 @@
       <c r="I10" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="2" t="s">
         <v>148</v>
       </c>
       <c r="M10">
@@ -1594,7 +1589,7 @@
       <c r="O10" t="s">
         <v>12</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10">
         <v>0</v>
       </c>
       <c r="Q10">
@@ -1614,13 +1609,13 @@
       <c r="C11" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G11">
@@ -1632,13 +1627,13 @@
       <c r="I11" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>149</v>
       </c>
       <c r="M11">
@@ -1650,7 +1645,7 @@
       <c r="O11" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11">
         <v>0</v>
       </c>
       <c r="Q11">
@@ -1670,13 +1665,13 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G12">
@@ -1685,16 +1680,16 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J12" s="3" t="s">
+      <c r="I12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M12">
@@ -1706,7 +1701,7 @@
       <c r="O12" t="s">
         <v>12</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
@@ -1726,13 +1721,13 @@
       <c r="C13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G13">
@@ -1744,7 +1739,7 @@
       <c r="I13" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K13">
@@ -1762,7 +1757,7 @@
       <c r="O13" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="8">
+      <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
@@ -1782,13 +1777,13 @@
       <c r="C14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G14">
@@ -1800,7 +1795,7 @@
       <c r="I14" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K14">
@@ -1818,7 +1813,7 @@
       <c r="O14" t="s">
         <v>12</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P14">
         <v>0</v>
       </c>
       <c r="Q14">
@@ -1838,13 +1833,13 @@
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G15">
@@ -1853,16 +1848,16 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J15" s="3" t="s">
+      <c r="I15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="L15" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M15">
@@ -1874,7 +1869,7 @@
       <c r="O15" t="s">
         <v>12</v>
       </c>
-      <c r="P15" s="8">
+      <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
@@ -1894,13 +1889,13 @@
       <c r="C16" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G16">
@@ -1912,7 +1907,7 @@
       <c r="I16" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K16">
@@ -1927,10 +1922,10 @@
       <c r="N16" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="5">
+      <c r="O16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16">
         <v>0</v>
       </c>
       <c r="Q16">
@@ -1950,13 +1945,13 @@
       <c r="C17" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G17">
@@ -1968,7 +1963,7 @@
       <c r="I17" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K17">
@@ -1986,7 +1981,7 @@
       <c r="O17" t="s">
         <v>12</v>
       </c>
-      <c r="P17" s="8">
+      <c r="P17">
         <v>0</v>
       </c>
       <c r="Q17">
@@ -2006,13 +2001,13 @@
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G18">
@@ -2021,16 +2016,16 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J18" s="3" t="s">
+      <c r="I18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M18">
@@ -2042,7 +2037,7 @@
       <c r="O18" t="s">
         <v>12</v>
       </c>
-      <c r="P18" s="8">
+      <c r="P18">
         <v>0</v>
       </c>
       <c r="Q18">
@@ -2062,13 +2057,13 @@
       <c r="C19" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G19">
@@ -2080,7 +2075,7 @@
       <c r="I19" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K19">
@@ -2098,7 +2093,7 @@
       <c r="O19" t="s">
         <v>12</v>
       </c>
-      <c r="P19" s="8">
+      <c r="P19">
         <v>0</v>
       </c>
       <c r="Q19">
@@ -2118,13 +2113,13 @@
       <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G20">
@@ -2136,7 +2131,7 @@
       <c r="I20" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K20">
@@ -2154,7 +2149,7 @@
       <c r="O20" t="s">
         <v>12</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20">
         <v>0</v>
       </c>
       <c r="Q20">
@@ -2174,13 +2169,13 @@
       <c r="C21" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G21">
@@ -2192,13 +2187,13 @@
       <c r="I21" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M21">
@@ -2210,7 +2205,7 @@
       <c r="O21" t="s">
         <v>12</v>
       </c>
-      <c r="P21" s="8">
+      <c r="P21">
         <v>0</v>
       </c>
       <c r="Q21">
@@ -2230,13 +2225,13 @@
       <c r="C22" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="D22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G22">
@@ -2248,13 +2243,13 @@
       <c r="I22" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M22">
@@ -2266,7 +2261,7 @@
       <c r="O22" t="s">
         <v>12</v>
       </c>
-      <c r="P22" s="8">
+      <c r="P22">
         <v>0</v>
       </c>
       <c r="Q22">
@@ -2286,13 +2281,13 @@
       <c r="C23" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G23">
@@ -2304,13 +2299,13 @@
       <c r="I23" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M23">
@@ -2319,10 +2314,10 @@
       <c r="N23" t="s">
         <v>12</v>
       </c>
-      <c r="O23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="P23" s="5">
+      <c r="O23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P23">
         <v>0</v>
       </c>
       <c r="Q23">
@@ -2342,13 +2337,13 @@
       <c r="C24" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G24">
@@ -2360,13 +2355,13 @@
       <c r="I24" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M24">
@@ -2378,7 +2373,7 @@
       <c r="O24" t="s">
         <v>12</v>
       </c>
-      <c r="P24" s="8">
+      <c r="P24">
         <v>0</v>
       </c>
       <c r="Q24">
@@ -2395,13 +2390,13 @@
       <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G25">
@@ -2413,13 +2408,13 @@
       <c r="I25" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K25">
         <v>1</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="L25" t="s">
         <v>112</v>
       </c>
       <c r="M25">
@@ -2431,7 +2426,7 @@
       <c r="O25" t="s">
         <v>12</v>
       </c>
-      <c r="P25" s="8">
+      <c r="P25">
         <v>0</v>
       </c>
       <c r="Q25">
@@ -2448,13 +2443,13 @@
       <c r="B26" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F26" s="3" t="s">
+      <c r="D26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G26">
@@ -2466,13 +2461,13 @@
       <c r="I26" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K26">
         <v>1</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" t="s">
         <v>111</v>
       </c>
       <c r="M26">
@@ -2484,7 +2479,7 @@
       <c r="O26" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="8">
+      <c r="P26">
         <v>0</v>
       </c>
       <c r="Q26">
@@ -2504,13 +2499,13 @@
       <c r="C27" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="3" t="s">
+      <c r="D27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G27" t="s">
@@ -2519,16 +2514,16 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J27" s="3" t="s">
+      <c r="I27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M27">
@@ -2537,10 +2532,10 @@
       <c r="N27" t="s">
         <v>118</v>
       </c>
-      <c r="O27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P27" s="8">
+      <c r="O27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P27">
         <v>0</v>
       </c>
       <c r="Q27" t="s">
@@ -2557,13 +2552,13 @@
       <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G28">
@@ -2572,28 +2567,28 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J28" s="3" t="s">
+      <c r="I28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M28">
         <v>1</v>
       </c>
-      <c r="N28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P28" s="8">
+      <c r="N28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P28">
         <v>0</v>
       </c>
       <c r="Q28">
@@ -2610,13 +2605,13 @@
       <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="D29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G29">
@@ -2625,28 +2620,28 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J29" s="3" t="s">
+      <c r="I29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M29">
         <v>1</v>
       </c>
-      <c r="N29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P29" s="8">
+      <c r="N29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P29">
         <v>0</v>
       </c>
       <c r="Q29">
@@ -2663,13 +2658,13 @@
       <c r="B30" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="D30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G30">
@@ -2678,16 +2673,16 @@
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J30" s="3" t="s">
+      <c r="I30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K30">
         <v>1</v>
       </c>
-      <c r="L30" s="8" t="s">
+      <c r="L30" t="s">
         <v>117</v>
       </c>
       <c r="M30">
@@ -2696,10 +2691,10 @@
       <c r="N30" t="s">
         <v>100</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P30" s="8">
+      <c r="O30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P30">
         <v>0</v>
       </c>
       <c r="Q30">
@@ -2719,31 +2714,31 @@
       <c r="C31" t="s">
         <v>126</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="D31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G31">
-        <v>1616</v>
+        <v>16</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="I31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K31">
         <v>1</v>
       </c>
-      <c r="L31" s="8" t="s">
+      <c r="L31" t="s">
         <v>199</v>
       </c>
       <c r="M31">
@@ -2752,10 +2747,10 @@
       <c r="N31" t="s">
         <v>12</v>
       </c>
-      <c r="O31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P31" s="8">
+      <c r="O31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31">
         <v>0</v>
       </c>
       <c r="Q31">
@@ -2775,13 +2770,13 @@
       <c r="C32" t="s">
         <v>128</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="D32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G32">
@@ -2790,16 +2785,16 @@
       <c r="H32">
         <v>1</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>100</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L32" t="s">
         <v>183</v>
       </c>
       <c r="M32">
@@ -2808,10 +2803,10 @@
       <c r="N32" t="s">
         <v>12</v>
       </c>
-      <c r="O32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P32" s="8">
+      <c r="O32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32">
         <v>0</v>
       </c>
       <c r="Q32">
@@ -2831,13 +2826,13 @@
       <c r="C33" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G33">
@@ -2846,13 +2841,13 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P33" s="8">
+      <c r="I33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P33">
         <v>0</v>
       </c>
       <c r="Q33">
@@ -2872,13 +2867,13 @@
       <c r="C34" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G34">
@@ -2887,13 +2882,13 @@
       <c r="H34">
         <v>0</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P34" s="8">
+      <c r="I34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P34">
         <v>0</v>
       </c>
       <c r="Q34">
@@ -2913,13 +2908,13 @@
       <c r="C35" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>100</v>
       </c>
       <c r="G35">
@@ -2928,13 +2923,13 @@
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="P35" s="8">
+      <c r="I35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P35">
         <v>0</v>
       </c>
       <c r="Q35">
@@ -2945,10 +2940,10 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F36" s="9"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F37" s="9"/>
+      <c r="F37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2978,7 +2973,7 @@
       <c r="C1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3098,7 +3093,7 @@
       <c r="H1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3198,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C76174-3001-4439-8CB8-D37020797EB5}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3797,7 +3792,7 @@
       <c r="C18" t="s">
         <v>113</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="5" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pewter dust and recipes
</commit_message>
<xml_diff>
--- a/.develop/ModAdditions.xlsx
+++ b/.develop/ModAdditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Documents\My Games\Terraria\tModLoader\ModSources\AllomancyMOD\.develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD5E838-C388-4E08-80A0-2F525A2518AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA0A50-F75F-43D4-A975-093DF486E6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="207">
   <si>
     <t>Title</t>
   </si>
@@ -643,6 +643,27 @@
   </si>
   <si>
     <t>re10 - re11</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
+  <si>
+    <t>re14</t>
+  </si>
+  <si>
+    <t>Workbench</t>
+  </si>
+  <si>
+    <t>re15</t>
+  </si>
+  <si>
+    <t>re16</t>
+  </si>
+  <si>
+    <t>re17</t>
   </si>
 </sst>
 </file>
@@ -1028,9 +1049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828CD007-B033-468F-8ADE-6460DAA113A1}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G32" sqref="G32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C32" sqref="C32:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3191,10 +3212,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C76174-3001-4439-8CB8-D37020797EB5}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,7 +3268,7 @@
         <v>150</v>
       </c>
       <c r="G2" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3270,7 +3291,7 @@
         <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3431,7 +3452,7 @@
         <v>150</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3454,7 +3475,7 @@
         <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3523,6 +3544,98 @@
         <v>150</v>
       </c>
       <c r="G14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" t="s">
+        <v>150</v>
+      </c>
+      <c r="G16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" t="s">
+        <v>150</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3536,7 +3649,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E22"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
metallurgy table - 1
</commit_message>
<xml_diff>
--- a/.develop/ModAdditions.xlsx
+++ b/.develop/ModAdditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Andriu\Documents\My Games\Terraria\tModLoader\ModSources\AllomancyMOD\.develop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEA0A50-F75F-43D4-A975-093DF486E6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33ACDF9-6497-4489-9C37-130DF8C84C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{3251149E-E61E-445A-8013-BC33DF00FE4F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEMS" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="207">
   <si>
     <t>Title</t>
   </si>
@@ -3215,7 +3215,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3498,7 +3498,7 @@
         <v>150</v>
       </c>
       <c r="G12" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3521,7 +3521,7 @@
         <v>150</v>
       </c>
       <c r="G13" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
         <v>150</v>
       </c>
       <c r="G14" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3646,10 +3646,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E8BBBC-6FA5-4E62-AC4D-14E3F43FDE97}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D20" sqref="A19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3917,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -3925,16 +3925,44 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>192</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>191</v>
-      </c>
-      <c r="D20">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D21">
         <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>